<commit_message>
Revamped , offer section added
</commit_message>
<xml_diff>
--- a/components/bulkOffer.xlsx
+++ b/components/bulkOffer.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25831"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="37" documentId="11_EE3A104055FD8542125FD718CC4B15AB53547A38" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{53C1D951-6695-439C-AA90-A8C23F64F657}"/>
+  <xr:revisionPtr revIDLastSave="61" documentId="11_EE3A104055FD8542125FD718CC4B15AB53547A38" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1E6A01E2-9236-4CDE-85DD-DBC6912755C8}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -15,39 +15,27 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>roll_no</t>
   </si>
   <si>
+    <t>company_name</t>
+  </si>
+  <si>
+    <t>package</t>
+  </si>
+  <si>
+    <t>role</t>
+  </si>
+  <si>
+    <t>TruckWawale</t>
+  </si>
+  <si>
+    <t>Data Analyst</t>
+  </si>
+  <si>
     <t>19IT1058</t>
-  </si>
-  <si>
-    <t>19IT1093</t>
-  </si>
-  <si>
-    <t>19IT2024</t>
-  </si>
-  <si>
-    <t>company_name</t>
-  </si>
-  <si>
-    <t>package</t>
-  </si>
-  <si>
-    <t>role</t>
-  </si>
-  <si>
-    <t>Big Data Analyst</t>
-  </si>
-  <si>
-    <t>BCS</t>
-  </si>
-  <si>
-    <t>Full Stack Developer</t>
-  </si>
-  <si>
-    <t>SDE</t>
   </si>
 </sst>
 </file>
@@ -428,10 +416,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -444,55 +432,27 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C2">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="D2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3">
-        <v>15</v>
-      </c>
-      <c r="D3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4">
-        <v>25</v>
-      </c>
-      <c r="D4" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>